<commit_message>
Today's work on Lucrare licenta
</commit_message>
<xml_diff>
--- a/docs/Registru1.xlsx
+++ b/docs/Registru1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="24">
   <si>
     <t>. . .</t>
   </si>
@@ -74,6 +74,21 @@
   <si>
     <t>a[1]</t>
   </si>
+  <si>
+    <t>x[n+1]</t>
+  </si>
+  <si>
+    <t>x[n+2]</t>
+  </si>
+  <si>
+    <t>b[4]</t>
+  </si>
+  <si>
+    <t>y[n+1]</t>
+  </si>
+  <si>
+    <t>y[n+2]</t>
+  </si>
 </sst>
 </file>
 
@@ -105,12 +120,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -162,15 +183,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -179,15 +197,25 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -219,7 +247,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2551606" y="1198689"/>
+          <a:off x="2571994" y="1197097"/>
           <a:ext cx="18722" cy="765220"/>
           <a:chOff x="1927860" y="1055372"/>
           <a:chExt cx="94922" cy="281939"/>
@@ -324,7 +352,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1978620" y="1201912"/>
+          <a:off x="1993911" y="1200320"/>
           <a:ext cx="314605" cy="754376"/>
           <a:chOff x="1927860" y="1055372"/>
           <a:chExt cx="94922" cy="281939"/>
@@ -429,7 +457,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1495043" y="1198684"/>
+          <a:off x="1505237" y="1197092"/>
           <a:ext cx="314605" cy="765219"/>
           <a:chOff x="1927860" y="1055372"/>
           <a:chExt cx="94922" cy="281939"/>
@@ -534,7 +562,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1011466" y="1198889"/>
+          <a:off x="1016563" y="1197297"/>
           <a:ext cx="312099" cy="768836"/>
           <a:chOff x="1927860" y="1055372"/>
           <a:chExt cx="94922" cy="281939"/>
@@ -702,7 +730,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm rot="10800000">
-          <a:off x="417476" y="3095233"/>
+          <a:off x="417476" y="3093641"/>
           <a:ext cx="312099" cy="393161"/>
           <a:chOff x="1927860" y="1055372"/>
           <a:chExt cx="94922" cy="281939"/>
@@ -807,7 +835,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm rot="10800000">
-          <a:off x="883219" y="3093058"/>
+          <a:off x="888316" y="3091466"/>
           <a:ext cx="312099" cy="393161"/>
           <a:chOff x="1927860" y="1055372"/>
           <a:chExt cx="94922" cy="281939"/>
@@ -1412,7 +1440,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm rot="10800000">
-          <a:off x="1380647" y="3093919"/>
+          <a:off x="1390841" y="3092327"/>
           <a:ext cx="312099" cy="393161"/>
           <a:chOff x="1927860" y="1055372"/>
           <a:chExt cx="94922" cy="281939"/>
@@ -1517,7 +1545,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm rot="10800000">
-          <a:off x="1853381" y="3090628"/>
+          <a:off x="1868672" y="3089036"/>
           <a:ext cx="312099" cy="393161"/>
           <a:chOff x="1927860" y="1055372"/>
           <a:chExt cx="94922" cy="281939"/>
@@ -1600,6 +1628,1864 @@
         </xdr:txBody>
       </xdr:sp>
     </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>247895</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>380431</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>266617</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>2651</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="37" name="Grupare 36"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="4057895" y="1192127"/>
+          <a:ext cx="18722" cy="765220"/>
+          <a:chOff x="1927860" y="1055372"/>
+          <a:chExt cx="94922" cy="281939"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="39" name="Conector drept cu săgeată 38"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000" flipH="1">
+            <a:off x="1817374" y="1196341"/>
+            <a:ext cx="281939" cy="1"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:tailEnd type="arrow"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="40" name="CasetăText 39"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1927860" y="1148535"/>
+            <a:ext cx="94922" cy="106728"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0" anchor="b">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="800"/>
+              <a:t>*</a:t>
+            </a:r>
+            <a:endParaRPr lang="ro-RO" sz="800"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>133638</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>2654</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>448243</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>376030</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="41" name="Grupare 40"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="5931464" y="1195350"/>
+          <a:ext cx="314605" cy="754376"/>
+          <a:chOff x="1927860" y="1055372"/>
+          <a:chExt cx="94922" cy="281939"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="42" name="Conector drept cu săgeată 41"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000" flipH="1">
+            <a:off x="1817374" y="1196341"/>
+            <a:ext cx="281939" cy="1"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:tailEnd type="arrow"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="43" name="CasetăText 42"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1927860" y="1146810"/>
+            <a:ext cx="94922" cy="108780"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0" anchor="b">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="800"/>
+              <a:t>*</a:t>
+            </a:r>
+            <a:endParaRPr lang="ro-RO" sz="800"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>141920</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>380426</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>456525</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>2645</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="44" name="Grupare 43"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="5442790" y="1192122"/>
+          <a:ext cx="314605" cy="765219"/>
+          <a:chOff x="1927860" y="1055372"/>
+          <a:chExt cx="94922" cy="281939"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="45" name="Conector drept cu săgeată 44"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000" flipH="1">
+            <a:off x="1817374" y="1196341"/>
+            <a:ext cx="281939" cy="1"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:tailEnd type="arrow"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="46" name="CasetăText 45"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1927860" y="1148538"/>
+            <a:ext cx="94922" cy="106728"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0" anchor="b">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="800"/>
+              <a:t>*</a:t>
+            </a:r>
+            <a:endParaRPr lang="ro-RO" sz="800"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>150203</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>380631</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>462302</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>6467</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="47" name="Grupare 46"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="4954116" y="1192327"/>
+          <a:ext cx="312099" cy="768836"/>
+          <a:chOff x="1927860" y="1055372"/>
+          <a:chExt cx="94922" cy="281939"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="48" name="Conector drept cu săgeată 47"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000" flipH="1">
+            <a:off x="1817374" y="1196341"/>
+            <a:ext cx="281939" cy="1"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:tailEnd type="arrow"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="49" name="CasetăText 48"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1927860" y="1145998"/>
+            <a:ext cx="94922" cy="106061"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0" anchor="b">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="800"/>
+              <a:t>*</a:t>
+            </a:r>
+            <a:endParaRPr lang="ro-RO" sz="800"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>178363</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>378684</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>492968</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>371060</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="51" name="Grupare 50"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="4485320" y="1190380"/>
+          <a:ext cx="314605" cy="754376"/>
+          <a:chOff x="1927860" y="1055372"/>
+          <a:chExt cx="94922" cy="281939"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="52" name="Conector drept cu săgeată 51"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000" flipH="1">
+            <a:off x="1817374" y="1196341"/>
+            <a:ext cx="281939" cy="1"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:tailEnd type="arrow"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="53" name="CasetăText 52"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1927860" y="1146810"/>
+            <a:ext cx="94922" cy="108780"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0" anchor="b">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="800"/>
+              <a:t>*</a:t>
+            </a:r>
+            <a:endParaRPr lang="ro-RO" sz="800"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>196959</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>304908</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="260969" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="54" name="CasetăText 53"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5994785" y="2640604"/>
+          <a:ext cx="260969" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ro-RO" sz="1100">
+              <a:latin typeface="+mn-lt"/>
+            </a:rPr>
+            <a:t>∑</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>255357</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>3002</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>255372</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>205664</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="55" name="Conector drept 54"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="5951860" y="2440021"/>
+          <a:ext cx="202662" cy="15"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>259584</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>378323</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>262032</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>201603</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="56" name="Conector drept 55"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="5459538" y="2433935"/>
+          <a:ext cx="204280" cy="2448"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>279230</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>3790</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>280818</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>206450</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="57" name="Conector drept 56"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="4982607" y="2440022"/>
+          <a:ext cx="202660" cy="1588"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>263997</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>205656</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>247173</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>206761</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="58" name="Conector drept 57"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4073997" y="2541352"/>
+          <a:ext cx="1971002" cy="1105"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>255632</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>201327</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>256762</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>8284</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="59" name="Conector drept 58"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="5769544" y="2820937"/>
+          <a:ext cx="568957" cy="1130"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>246332</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>636</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>248780</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>204916</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="61" name="Conector drept 60"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="4452373" y="2437248"/>
+          <a:ext cx="204280" cy="2448"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>265978</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>7103</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>267566</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>209763</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="62" name="Conector drept 61"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="3975442" y="2443335"/>
+          <a:ext cx="202660" cy="1588"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>214764</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>380431</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>233486</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>2651</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="63" name="Grupare 62"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="11479112" y="1192127"/>
+          <a:ext cx="18722" cy="765220"/>
+          <a:chOff x="1927860" y="1055372"/>
+          <a:chExt cx="94922" cy="281939"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="64" name="Conector drept cu săgeată 63"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000" flipH="1">
+            <a:off x="1817374" y="1196341"/>
+            <a:ext cx="281939" cy="1"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:tailEnd type="arrow"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="65" name="CasetăText 64"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1927860" y="1148535"/>
+            <a:ext cx="94922" cy="106728"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0" anchor="b">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="800"/>
+              <a:t>*</a:t>
+            </a:r>
+            <a:endParaRPr lang="ro-RO" sz="800"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>133638</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>2654</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>448243</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>376030</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="66" name="Grupare 65"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="10901029" y="1195350"/>
+          <a:ext cx="314605" cy="754376"/>
+          <a:chOff x="1927860" y="1055372"/>
+          <a:chExt cx="94922" cy="281939"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="67" name="Conector drept cu săgeată 66"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000" flipH="1">
+            <a:off x="1817374" y="1196341"/>
+            <a:ext cx="281939" cy="1"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:tailEnd type="arrow"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="68" name="CasetăText 67"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1927860" y="1146810"/>
+            <a:ext cx="94922" cy="108780"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0" anchor="b">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="800"/>
+              <a:t>*</a:t>
+            </a:r>
+            <a:endParaRPr lang="ro-RO" sz="800"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>141920</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>380426</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>456525</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>2645</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="69" name="Grupare 68"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="10412355" y="1192122"/>
+          <a:ext cx="314605" cy="765219"/>
+          <a:chOff x="1927860" y="1055372"/>
+          <a:chExt cx="94922" cy="281939"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="70" name="Conector drept cu săgeată 69"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000" flipH="1">
+            <a:off x="1817374" y="1196341"/>
+            <a:ext cx="281939" cy="1"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:tailEnd type="arrow"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="71" name="CasetăText 70"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1927860" y="1148538"/>
+            <a:ext cx="94922" cy="106728"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0" anchor="b">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="800"/>
+              <a:t>*</a:t>
+            </a:r>
+            <a:endParaRPr lang="ro-RO" sz="800"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>150203</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>380631</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>462302</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>6467</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="72" name="Grupare 71"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="9923681" y="1192327"/>
+          <a:ext cx="312099" cy="768836"/>
+          <a:chOff x="1927860" y="1055372"/>
+          <a:chExt cx="94922" cy="281939"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="73" name="Conector drept cu săgeată 72"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000" flipH="1">
+            <a:off x="1817374" y="1196341"/>
+            <a:ext cx="281939" cy="1"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:tailEnd type="arrow"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="74" name="CasetăText 73"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1927860" y="1145998"/>
+            <a:ext cx="94922" cy="106061"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0" anchor="b">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="800"/>
+              <a:t>*</a:t>
+            </a:r>
+            <a:endParaRPr lang="ro-RO" sz="800"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>145233</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>378684</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>459838</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>371060</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="75" name="Grupare 74"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="11906537" y="1190380"/>
+          <a:ext cx="314605" cy="754376"/>
+          <a:chOff x="1927860" y="1055372"/>
+          <a:chExt cx="94922" cy="281939"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="76" name="Conector drept cu săgeată 75"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000" flipH="1">
+            <a:off x="1817374" y="1196341"/>
+            <a:ext cx="281939" cy="1"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:tailEnd type="arrow"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="77" name="CasetăText 76"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1927860" y="1146810"/>
+            <a:ext cx="94922" cy="108780"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0" anchor="b">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="800"/>
+              <a:t>*</a:t>
+            </a:r>
+            <a:endParaRPr lang="ro-RO" sz="800"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>196959</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>304908</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="260969" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="78" name="CasetăText 77"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5994785" y="2640604"/>
+          <a:ext cx="260969" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ro-RO" sz="1100">
+              <a:latin typeface="+mn-lt"/>
+            </a:rPr>
+            <a:t>∑</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>255357</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>3002</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>255372</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>205664</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="79" name="Conector drept 78"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="5951860" y="2440021"/>
+          <a:ext cx="202662" cy="15"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>259584</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>378323</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>262032</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>201603</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="80" name="Conector drept 79"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="5459538" y="2433935"/>
+          <a:ext cx="204280" cy="2448"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>279230</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>3790</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>280818</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>206450</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="81" name="Conector drept 80"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="4982607" y="2440022"/>
+          <a:ext cx="202660" cy="1588"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>280563</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>205656</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>263739</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>206761</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="82" name="Conector drept 81"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5084476" y="2541352"/>
+          <a:ext cx="1971002" cy="1105"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>255632</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>201327</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>256762</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>8284</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="83" name="Conector drept 82"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="5769544" y="2820937"/>
+          <a:ext cx="568957" cy="1130"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>262898</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>636</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>265346</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>204916</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="84" name="Conector drept 83"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="6953721" y="2437248"/>
+          <a:ext cx="204280" cy="2448"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>282543</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>7103</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>284131</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>209763</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="85" name="Conector drept 84"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="6476790" y="2443335"/>
+          <a:ext cx="202660" cy="1588"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1917,170 +3803,405 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A4:N12"/>
+  <dimension ref="A4:AA12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.7109375" style="1" customWidth="1"/>
     <col min="2" max="7" width="7.28515625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="7.42578125" style="1" customWidth="1"/>
-    <col min="9" max="14" width="2.85546875" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="1"/>
+    <col min="8" max="26" width="7.42578125" style="1" customWidth="1"/>
+    <col min="27" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:14" ht="18.75">
+    <row r="4" spans="1:27" ht="18.75">
       <c r="A4" s="3"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="10"/>
+      <c r="U4" s="10"/>
+      <c r="V4" s="10"/>
+      <c r="W4" s="10"/>
+      <c r="X4" s="10"/>
+      <c r="Y4" s="10"/>
+      <c r="Z4" s="10"/>
+      <c r="AA4" s="10"/>
     </row>
-    <row r="5" spans="1:14" ht="30" customHeight="1">
+    <row r="5" spans="1:27" ht="30" customHeight="1">
       <c r="A5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="8"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="M5" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="N5" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="O5" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="P5" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="S5" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="T5" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="U5" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="V5" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="W5" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="X5" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y5" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z5" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="10"/>
     </row>
-    <row r="6" spans="1:14" ht="30" customHeight="1">
+    <row r="6" spans="1:27" ht="30" customHeight="1">
       <c r="A6" s="3"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="11"/>
+      <c r="S6" s="11"/>
+      <c r="T6" s="11"/>
+      <c r="U6" s="11"/>
+      <c r="V6" s="11"/>
+      <c r="W6" s="11"/>
+      <c r="X6" s="11"/>
+      <c r="Y6" s="11"/>
+      <c r="Z6" s="11"/>
+      <c r="AA6" s="10"/>
     </row>
-    <row r="7" spans="1:14" ht="30" customHeight="1">
+    <row r="7" spans="1:27" ht="30" customHeight="1">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="11"/>
+      <c r="S7" s="11"/>
+      <c r="T7" s="11"/>
+      <c r="U7" s="11"/>
+      <c r="V7" s="11"/>
+      <c r="W7" s="11"/>
+      <c r="X7" s="11"/>
+      <c r="Y7" s="11"/>
+      <c r="Z7" s="11"/>
+      <c r="AA7" s="10"/>
     </row>
-    <row r="8" spans="1:14" ht="30" customHeight="1">
+    <row r="8" spans="1:27" ht="30" customHeight="1">
       <c r="A8" s="3"/>
       <c r="B8" s="4"/>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="K8" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="L8" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="M8" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="11"/>
+      <c r="S8" s="11"/>
+      <c r="T8" s="11"/>
+      <c r="U8" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="V8" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="W8" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="X8" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y8" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z8" s="11"/>
+      <c r="AA8" s="10"/>
     </row>
-    <row r="9" spans="1:14" ht="30" customHeight="1">
+    <row r="9" spans="1:27" ht="30" customHeight="1">
       <c r="A9" s="3"/>
       <c r="B9" s="4"/>
       <c r="D9" s="1"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="11"/>
+      <c r="S9" s="11"/>
+      <c r="T9" s="11"/>
+      <c r="U9" s="11"/>
+      <c r="V9" s="11"/>
+      <c r="W9" s="11"/>
+      <c r="X9" s="11"/>
+      <c r="Y9" s="11"/>
+      <c r="Z9" s="11"/>
+      <c r="AA9" s="10"/>
     </row>
-    <row r="10" spans="1:14" ht="30" customHeight="1">
+    <row r="10" spans="1:27" ht="30" customHeight="1">
       <c r="A10" s="3"/>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="7" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="1"/>
-      <c r="G10" s="12"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="11"/>
+      <c r="S10" s="11"/>
+      <c r="T10" s="11"/>
+      <c r="U10" s="11"/>
+      <c r="V10" s="11"/>
+      <c r="W10" s="11"/>
+      <c r="X10" s="11"/>
+      <c r="Y10" s="11"/>
+      <c r="Z10" s="11"/>
+      <c r="AA10" s="10"/>
     </row>
-    <row r="11" spans="1:14" ht="30" customHeight="1">
-      <c r="H11" s="9"/>
-      <c r="I11" s="10"/>
+    <row r="11" spans="1:27" ht="30" customHeight="1">
+      <c r="G11" s="14"/>
+      <c r="H11" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="J11" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="L11" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="M11" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="N11" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="O11" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="P11" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="10"/>
+      <c r="R11" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="S11" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="T11" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="U11" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="V11" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="W11" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="X11" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y11" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z11" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="10"/>
     </row>
-    <row r="12" spans="1:14" ht="30" customHeight="1">
+    <row r="12" spans="1:27" ht="30" customHeight="1">
       <c r="A12" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="8"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="10"/>
+      <c r="S12" s="10"/>
+      <c r="T12" s="10"/>
+      <c r="U12" s="10"/>
+      <c r="V12" s="10"/>
+      <c r="W12" s="10"/>
+      <c r="X12" s="10"/>
+      <c r="Y12" s="10"/>
+      <c r="Z12" s="10"/>
+      <c r="AA12" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
AI changes and some Java package moves
</commit_message>
<xml_diff>
--- a/docs/Registru1.xlsx
+++ b/docs/Registru1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="14295" windowHeight="4620"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="14295" windowHeight="4620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Foaie1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="25">
   <si>
     <t>. . .</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>y[n+2]</t>
+  </si>
+  <si>
+    <t>a[0]</t>
   </si>
 </sst>
 </file>
@@ -183,7 +186,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -216,6 +219,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -247,7 +256,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2571994" y="1197097"/>
+          <a:off x="2560398" y="1195026"/>
           <a:ext cx="18722" cy="765220"/>
           <a:chOff x="1927860" y="1055372"/>
           <a:chExt cx="94922" cy="281939"/>
@@ -352,7 +361,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1993911" y="1200320"/>
+          <a:off x="1985214" y="1198249"/>
           <a:ext cx="314605" cy="754376"/>
           <a:chOff x="1927860" y="1055372"/>
           <a:chExt cx="94922" cy="281939"/>
@@ -457,7 +466,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1505237" y="1197092"/>
+          <a:off x="1499439" y="1195021"/>
           <a:ext cx="314605" cy="765219"/>
           <a:chOff x="1927860" y="1055372"/>
           <a:chExt cx="94922" cy="281939"/>
@@ -562,7 +571,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1016563" y="1197297"/>
+          <a:off x="1013664" y="1195226"/>
           <a:ext cx="312099" cy="768836"/>
           <a:chOff x="1927860" y="1055372"/>
           <a:chExt cx="94922" cy="281939"/>
@@ -730,7 +739,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm rot="10800000">
-          <a:off x="417476" y="3093641"/>
+          <a:off x="417476" y="3091570"/>
           <a:ext cx="312099" cy="393161"/>
           <a:chOff x="1927860" y="1055372"/>
           <a:chExt cx="94922" cy="281939"/>
@@ -835,7 +844,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm rot="10800000">
-          <a:off x="888316" y="3091466"/>
+          <a:off x="885417" y="3089395"/>
           <a:ext cx="312099" cy="393161"/>
           <a:chOff x="1927860" y="1055372"/>
           <a:chExt cx="94922" cy="281939"/>
@@ -1440,7 +1449,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm rot="10800000">
-          <a:off x="1390841" y="3092327"/>
+          <a:off x="1385043" y="3090256"/>
           <a:ext cx="312099" cy="393161"/>
           <a:chOff x="1927860" y="1055372"/>
           <a:chExt cx="94922" cy="281939"/>
@@ -1545,7 +1554,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm rot="10800000">
-          <a:off x="1868672" y="3089036"/>
+          <a:off x="1859975" y="3086965"/>
           <a:ext cx="312099" cy="393161"/>
           <a:chOff x="1927860" y="1055372"/>
           <a:chExt cx="94922" cy="281939"/>
@@ -1650,7 +1659,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4057895" y="1192127"/>
+          <a:off x="4038845" y="1190056"/>
           <a:ext cx="18722" cy="765220"/>
           <a:chOff x="1927860" y="1055372"/>
           <a:chExt cx="94922" cy="281939"/>
@@ -1755,7 +1764,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5931464" y="1195350"/>
+          <a:off x="5905788" y="1193279"/>
           <a:ext cx="314605" cy="754376"/>
           <a:chOff x="1927860" y="1055372"/>
           <a:chExt cx="94922" cy="281939"/>
@@ -1860,7 +1869,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5442790" y="1192122"/>
+          <a:off x="5418770" y="1190051"/>
           <a:ext cx="314605" cy="765219"/>
           <a:chOff x="1927860" y="1055372"/>
           <a:chExt cx="94922" cy="281939"/>
@@ -1965,7 +1974,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4954116" y="1192327"/>
+          <a:off x="4931753" y="1190256"/>
           <a:ext cx="312099" cy="768836"/>
           <a:chOff x="1927860" y="1055372"/>
           <a:chExt cx="94922" cy="281939"/>
@@ -2070,7 +2079,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4485320" y="1190380"/>
+          <a:off x="4464613" y="1188309"/>
           <a:ext cx="314605" cy="754376"/>
           <a:chOff x="1927860" y="1055372"/>
           <a:chExt cx="94922" cy="281939"/>
@@ -2579,7 +2588,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="11479112" y="1192127"/>
+          <a:off x="11435214" y="1190056"/>
           <a:ext cx="18722" cy="765220"/>
           <a:chOff x="1927860" y="1055372"/>
           <a:chExt cx="94922" cy="281939"/>
@@ -2684,7 +2693,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="10901029" y="1195350"/>
+          <a:off x="10858788" y="1193279"/>
           <a:ext cx="314605" cy="754376"/>
           <a:chOff x="1927860" y="1055372"/>
           <a:chExt cx="94922" cy="281939"/>
@@ -2789,7 +2798,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="10412355" y="1192122"/>
+          <a:off x="10371770" y="1190051"/>
           <a:ext cx="314605" cy="765219"/>
           <a:chOff x="1927860" y="1055372"/>
           <a:chExt cx="94922" cy="281939"/>
@@ -2894,7 +2903,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="9923681" y="1192327"/>
+          <a:off x="9884753" y="1190256"/>
           <a:ext cx="312099" cy="768836"/>
           <a:chOff x="1927860" y="1055372"/>
           <a:chExt cx="94922" cy="281939"/>
@@ -2999,7 +3008,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="11906537" y="1190380"/>
+          <a:off x="11860983" y="1188309"/>
           <a:ext cx="314605" cy="754376"/>
           <a:chOff x="1927860" y="1055372"/>
           <a:chExt cx="94922" cy="281939"/>
@@ -3459,6 +3468,2798 @@
       <xdr:spPr>
         <a:xfrm rot="5400000">
           <a:off x="6476790" y="2443335"/>
+          <a:ext cx="202660" cy="1588"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>247895</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>2651</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="171" name="Grupare 170"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1244357" y="771525"/>
+          <a:ext cx="66430" cy="755126"/>
+          <a:chOff x="1927860" y="1055372"/>
+          <a:chExt cx="94922" cy="281939"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="172" name="Conector drept cu săgeată 171"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000" flipH="1">
+            <a:off x="1817374" y="1196341"/>
+            <a:ext cx="281939" cy="1"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:tailEnd type="arrow"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="173" name="CasetăText 172"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1927860" y="1148535"/>
+            <a:ext cx="94922" cy="106728"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0" anchor="b">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="800"/>
+              <a:t>*</a:t>
+            </a:r>
+            <a:endParaRPr lang="ro-RO" sz="800"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>133638</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>2654</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>448243</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>4555</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="174" name="Grupare 173"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="3123023" y="764654"/>
+          <a:ext cx="314605" cy="763901"/>
+          <a:chOff x="1927860" y="1055372"/>
+          <a:chExt cx="94922" cy="281939"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="175" name="Conector drept cu săgeată 174"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000" flipH="1">
+            <a:off x="1817374" y="1196341"/>
+            <a:ext cx="281939" cy="1"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:tailEnd type="arrow"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="176" name="CasetăText 175"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1927860" y="1146810"/>
+            <a:ext cx="94922" cy="108780"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0" anchor="b">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="800"/>
+              <a:t>*</a:t>
+            </a:r>
+            <a:endParaRPr lang="ro-RO" sz="800"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>141920</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>371474</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>456525</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>2645</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="177" name="Grupare 176"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="2633074" y="752474"/>
+          <a:ext cx="314605" cy="774171"/>
+          <a:chOff x="1927860" y="1055372"/>
+          <a:chExt cx="94922" cy="281939"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="178" name="Conector drept cu săgeată 177"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000" flipH="1">
+            <a:off x="1817374" y="1196341"/>
+            <a:ext cx="281939" cy="1"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:tailEnd type="arrow"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="179" name="CasetăText 178"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1927860" y="1148538"/>
+            <a:ext cx="94922" cy="106728"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0" anchor="b">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="800"/>
+              <a:t>*</a:t>
+            </a:r>
+            <a:endParaRPr lang="ro-RO" sz="800"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>150203</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>380999</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>462302</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>6466</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="180" name="Grupare 179"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="2143126" y="761999"/>
+          <a:ext cx="312099" cy="768467"/>
+          <a:chOff x="1927860" y="1055372"/>
+          <a:chExt cx="94922" cy="281939"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="181" name="Conector drept cu săgeată 180"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000" flipH="1">
+            <a:off x="1817374" y="1196341"/>
+            <a:ext cx="281939" cy="1"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:tailEnd type="arrow"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="182" name="CasetăText 181"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1927860" y="1145998"/>
+            <a:ext cx="94922" cy="106061"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0" anchor="b">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="800"/>
+              <a:t>*</a:t>
+            </a:r>
+            <a:endParaRPr lang="ro-RO" sz="800"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>178363</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>369159</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>492968</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>371060</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="183" name="Grupare 182"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1673055" y="750159"/>
+          <a:ext cx="314605" cy="763901"/>
+          <a:chOff x="1927860" y="1055372"/>
+          <a:chExt cx="94922" cy="281939"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="184" name="Conector drept cu săgeată 183"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000" flipH="1">
+            <a:off x="1817374" y="1196341"/>
+            <a:ext cx="281939" cy="1"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:tailEnd type="arrow"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="185" name="CasetăText 184"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1927860" y="1146810"/>
+            <a:ext cx="94922" cy="108780"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0" anchor="b">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="800"/>
+              <a:t>*</a:t>
+            </a:r>
+            <a:endParaRPr lang="ro-RO" sz="800"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>196959</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>304908</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="260969" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="186" name="CasetăText 185"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5969109" y="2638533"/>
+          <a:ext cx="260969" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ro-RO" sz="1100">
+              <a:latin typeface="+mn-lt"/>
+            </a:rPr>
+            <a:t>∑</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>255357</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>3002</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>255372</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>205664</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="187" name="Conector drept 186"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="5926184" y="2437950"/>
+          <a:ext cx="202662" cy="15"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>259584</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>378323</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>262032</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>201603</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="188" name="Conector drept 187"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="5435518" y="2431864"/>
+          <a:ext cx="204280" cy="2448"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>279230</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>3790</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>280818</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>206450</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="189" name="Conector drept 188"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="4960244" y="2437951"/>
+          <a:ext cx="202660" cy="1588"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>263997</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>205656</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>247173</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>206761</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="190" name="Conector drept 189"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4054947" y="2539281"/>
+          <a:ext cx="1964376" cy="1105"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>255632</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>201327</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>256762</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>8284</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="191" name="Conector drept 190"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="5743868" y="2818866"/>
+          <a:ext cx="568957" cy="1130"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>246332</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>636</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>248780</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>204916</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="192" name="Conector drept 191"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="4431666" y="2435177"/>
+          <a:ext cx="204280" cy="2448"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>265978</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>7103</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>267566</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>209763</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="193" name="Conector drept 192"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="3956392" y="2441264"/>
+          <a:ext cx="202660" cy="1588"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>247895</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>2651</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="194" name="Grupare 193"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="5230203" y="771525"/>
+          <a:ext cx="66430" cy="755126"/>
+          <a:chOff x="1927860" y="1055372"/>
+          <a:chExt cx="94922" cy="281939"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="195" name="Conector drept cu săgeată 194"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000" flipH="1">
+            <a:off x="1817374" y="1196341"/>
+            <a:ext cx="281939" cy="1"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:tailEnd type="arrow"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="196" name="CasetăText 195"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1927860" y="1148535"/>
+            <a:ext cx="94922" cy="106728"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0" anchor="b">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="800"/>
+              <a:t>*</a:t>
+            </a:r>
+            <a:endParaRPr lang="ro-RO" sz="800"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>133638</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>2654</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>448243</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>4555</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="197" name="Grupare 196"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="7108869" y="764654"/>
+          <a:ext cx="314605" cy="763901"/>
+          <a:chOff x="1927860" y="1055372"/>
+          <a:chExt cx="94922" cy="281939"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="198" name="Conector drept cu săgeată 197"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000" flipH="1">
+            <a:off x="1817374" y="1196341"/>
+            <a:ext cx="281939" cy="1"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:tailEnd type="arrow"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="199" name="CasetăText 198"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1927860" y="1146810"/>
+            <a:ext cx="94922" cy="108780"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0" anchor="b">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="800"/>
+              <a:t>*</a:t>
+            </a:r>
+            <a:endParaRPr lang="ro-RO" sz="800"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>141920</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>371474</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>456525</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>2645</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="200" name="Grupare 199"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="6618920" y="752474"/>
+          <a:ext cx="314605" cy="774171"/>
+          <a:chOff x="1927860" y="1055372"/>
+          <a:chExt cx="94922" cy="281939"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="201" name="Conector drept cu săgeată 200"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000" flipH="1">
+            <a:off x="1817374" y="1196341"/>
+            <a:ext cx="281939" cy="1"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:tailEnd type="arrow"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="202" name="CasetăText 201"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1927860" y="1148538"/>
+            <a:ext cx="94922" cy="106728"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0" anchor="b">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="800"/>
+              <a:t>*</a:t>
+            </a:r>
+            <a:endParaRPr lang="ro-RO" sz="800"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>150203</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>380999</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>462302</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>6466</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="203" name="Grupare 202"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="6128972" y="761999"/>
+          <a:ext cx="312099" cy="768467"/>
+          <a:chOff x="1927860" y="1055372"/>
+          <a:chExt cx="94922" cy="281939"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="204" name="Conector drept cu săgeată 203"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000" flipH="1">
+            <a:off x="1817374" y="1196341"/>
+            <a:ext cx="281939" cy="1"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:tailEnd type="arrow"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="205" name="CasetăText 204"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1927860" y="1145998"/>
+            <a:ext cx="94922" cy="106061"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0" anchor="b">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="800"/>
+              <a:t>*</a:t>
+            </a:r>
+            <a:endParaRPr lang="ro-RO" sz="800"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>178363</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>369159</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>492968</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>371060</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="206" name="Grupare 205"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="5658901" y="750159"/>
+          <a:ext cx="314605" cy="763901"/>
+          <a:chOff x="1927860" y="1055372"/>
+          <a:chExt cx="94922" cy="281939"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="207" name="Conector drept cu săgeată 206"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000" flipH="1">
+            <a:off x="1817374" y="1196341"/>
+            <a:ext cx="281939" cy="1"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:tailEnd type="arrow"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="208" name="CasetăText 207"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1927860" y="1146810"/>
+            <a:ext cx="94922" cy="108780"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0" anchor="b">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="800"/>
+              <a:t>*</a:t>
+            </a:r>
+            <a:endParaRPr lang="ro-RO" sz="800"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>196959</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>304908</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="260969" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="209" name="CasetăText 208"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3155312" y="2209908"/>
+          <a:ext cx="260969" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ro-RO" sz="1100">
+              <a:latin typeface="+mn-lt"/>
+            </a:rPr>
+            <a:t>∑</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>255357</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>3002</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>255372</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>205664</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="210" name="Conector drept 209"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="3112387" y="2009325"/>
+          <a:ext cx="202662" cy="15"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>259584</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>378323</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>262032</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>201603</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="211" name="Conector drept 210"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="2623962" y="2003239"/>
+          <a:ext cx="204280" cy="2448"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>279230</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>3790</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>280818</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>206450</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="212" name="Conector drept 211"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="2150929" y="2009326"/>
+          <a:ext cx="202660" cy="1588"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>263997</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>205656</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>247173</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>206761</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="213" name="Conector drept 212"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1250115" y="2110656"/>
+          <a:ext cx="1955411" cy="1105"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>255632</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>201327</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>256762</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>8284</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="214" name="Conector drept 213"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="2930071" y="2390241"/>
+          <a:ext cx="568957" cy="1130"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>246332</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>636</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>248780</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>204916</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="215" name="Conector drept 214"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="1624592" y="2006552"/>
+          <a:ext cx="204280" cy="2448"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>265978</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>7103</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>267566</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>209763</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="216" name="Conector drept 215"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="1151560" y="2012639"/>
+          <a:ext cx="202660" cy="1588"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>247895</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>2651</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="217" name="Grupare 216"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="9714280" y="771525"/>
+          <a:ext cx="66430" cy="755126"/>
+          <a:chOff x="1927860" y="1055372"/>
+          <a:chExt cx="94922" cy="281939"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="218" name="Conector drept cu săgeată 217"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000" flipH="1">
+            <a:off x="1817374" y="1196341"/>
+            <a:ext cx="281939" cy="1"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:tailEnd type="arrow"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="219" name="CasetăText 218"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1927860" y="1148535"/>
+            <a:ext cx="94922" cy="106728"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0" anchor="b">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="800"/>
+              <a:t>*</a:t>
+            </a:r>
+            <a:endParaRPr lang="ro-RO" sz="800"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>133638</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>2654</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>448243</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>4555</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="220" name="Grupare 219"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="11922657" y="764654"/>
+          <a:ext cx="314605" cy="763901"/>
+          <a:chOff x="1927860" y="1055372"/>
+          <a:chExt cx="94922" cy="281939"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="221" name="Conector drept cu săgeată 220"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000" flipH="1">
+            <a:off x="1817374" y="1196341"/>
+            <a:ext cx="281939" cy="1"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:tailEnd type="arrow"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="222" name="CasetăText 221"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1927860" y="1146810"/>
+            <a:ext cx="94922" cy="108780"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0" anchor="b">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="800"/>
+              <a:t>*</a:t>
+            </a:r>
+            <a:endParaRPr lang="ro-RO" sz="800"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>141920</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>371474</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>456525</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>2645</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="223" name="Grupare 222"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="11322805" y="752474"/>
+          <a:ext cx="314605" cy="774171"/>
+          <a:chOff x="1927860" y="1055372"/>
+          <a:chExt cx="94922" cy="281939"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="224" name="Conector drept cu săgeată 223"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000" flipH="1">
+            <a:off x="1817374" y="1196341"/>
+            <a:ext cx="281939" cy="1"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:tailEnd type="arrow"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="225" name="CasetăText 224"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1927860" y="1148538"/>
+            <a:ext cx="94922" cy="106728"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0" anchor="b">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="800"/>
+              <a:t>*</a:t>
+            </a:r>
+            <a:endParaRPr lang="ro-RO" sz="800"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>150203</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>380999</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>462302</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>6466</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="226" name="Grupare 225"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="10722953" y="761999"/>
+          <a:ext cx="312099" cy="768467"/>
+          <a:chOff x="1927860" y="1055372"/>
+          <a:chExt cx="94922" cy="281939"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="227" name="Conector drept cu săgeată 226"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000" flipH="1">
+            <a:off x="1817374" y="1196341"/>
+            <a:ext cx="281939" cy="1"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:tailEnd type="arrow"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="228" name="CasetăText 227"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1927860" y="1145998"/>
+            <a:ext cx="94922" cy="106061"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0" anchor="b">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="800"/>
+              <a:t>*</a:t>
+            </a:r>
+            <a:endParaRPr lang="ro-RO" sz="800"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>178363</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>369159</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>492968</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>371060</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="229" name="Grupare 228"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="10142978" y="750159"/>
+          <a:ext cx="314605" cy="763901"/>
+          <a:chOff x="1927860" y="1055372"/>
+          <a:chExt cx="94922" cy="281939"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="230" name="Conector drept cu săgeată 229"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000" flipH="1">
+            <a:off x="1817374" y="1196341"/>
+            <a:ext cx="281939" cy="1"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:tailEnd type="arrow"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="231" name="CasetăText 230"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1927860" y="1146810"/>
+            <a:ext cx="94922" cy="108780"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0" anchor="b">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="800"/>
+              <a:t>*</a:t>
+            </a:r>
+            <a:endParaRPr lang="ro-RO" sz="800"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>196959</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>304908</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="260969" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="232" name="CasetăText 231"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7099783" y="2209908"/>
+          <a:ext cx="260969" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="ro-RO" sz="1100">
+              <a:latin typeface="+mn-lt"/>
+            </a:rPr>
+            <a:t>∑</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>255357</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>3002</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>255372</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>205664</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="233" name="Conector drept 232"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="7056858" y="2009325"/>
+          <a:ext cx="202662" cy="15"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>259584</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>378323</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>262032</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>201603</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="234" name="Conector drept 233"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="6568433" y="2003239"/>
+          <a:ext cx="204280" cy="2448"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>279230</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>3790</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>280818</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>206450</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="235" name="Conector drept 234"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="6095400" y="2009326"/>
+          <a:ext cx="202660" cy="1588"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>263997</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>205656</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>247173</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>206761</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="236" name="Conector drept 235"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5194585" y="2110656"/>
+          <a:ext cx="1955412" cy="1105"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>255632</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>201327</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>256762</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>8284</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="237" name="Conector drept 236"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="6874542" y="2390241"/>
+          <a:ext cx="568957" cy="1130"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>246332</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>636</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>248780</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>204916</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="238" name="Conector drept 237"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="5569063" y="2006552"/>
+          <a:ext cx="204280" cy="2448"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>265978</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>7103</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>267566</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>209763</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="239" name="Conector drept 238"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="5096030" y="2012639"/>
           <a:ext cx="202660" cy="1588"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -3805,8 +6606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A4:AA12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3999,19 +6800,19 @@
       <c r="G8" s="14"/>
       <c r="H8" s="11"/>
       <c r="I8" s="9" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="J8" s="9" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="L8" s="9" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="M8" s="9" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="N8" s="10"/>
       <c r="O8" s="10"/>
@@ -4212,13 +7013,377 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:Y9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="V18" sqref="V18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="20" width="7.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" ht="30" customHeight="1">
+      <c r="A1" s="12"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
+      <c r="W1" s="10"/>
+      <c r="X1" s="10"/>
+      <c r="Y1" s="10"/>
+    </row>
+    <row r="2" spans="1:25" ht="30" customHeight="1">
+      <c r="A2" s="13"/>
+      <c r="B2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="17"/>
+      <c r="I2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="N2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="O2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="P2" s="10"/>
+      <c r="Q2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="R2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="S2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="T2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="U2" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="V2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="W2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="X2" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y2" s="10"/>
+    </row>
+    <row r="3" spans="1:25" ht="30" customHeight="1">
+      <c r="A3" s="14"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="11"/>
+      <c r="U3" s="11"/>
+      <c r="V3" s="11"/>
+      <c r="W3" s="11"/>
+      <c r="X3" s="11"/>
+      <c r="Y3" s="10"/>
+    </row>
+    <row r="4" spans="1:25" ht="30" customHeight="1">
+      <c r="A4" s="14"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="11"/>
+      <c r="U4" s="11"/>
+      <c r="V4" s="11"/>
+      <c r="W4" s="11"/>
+      <c r="X4" s="11"/>
+      <c r="Y4" s="10"/>
+    </row>
+    <row r="5" spans="1:25" ht="30" customHeight="1">
+      <c r="A5" s="14"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="10"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="M5" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="N5" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="O5" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="11"/>
+      <c r="R5" s="10"/>
+      <c r="S5" s="10"/>
+      <c r="T5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="U5" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="V5" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="W5" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="X5" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y5" s="10"/>
+    </row>
+    <row r="6" spans="1:25" ht="30" customHeight="1">
+      <c r="A6" s="12"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="10"/>
+      <c r="S6" s="10"/>
+      <c r="T6" s="11"/>
+      <c r="U6" s="11"/>
+      <c r="V6" s="11"/>
+      <c r="W6" s="11"/>
+      <c r="X6" s="11"/>
+      <c r="Y6" s="10"/>
+    </row>
+    <row r="7" spans="1:25" ht="30" customHeight="1">
+      <c r="A7" s="15"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="11"/>
+      <c r="R7" s="10"/>
+      <c r="T7" s="11"/>
+      <c r="U7" s="11"/>
+      <c r="V7" s="11"/>
+      <c r="W7" s="11"/>
+      <c r="X7" s="11"/>
+      <c r="Y7" s="10"/>
+    </row>
+    <row r="8" spans="1:25" ht="30" customHeight="1">
+      <c r="A8" s="14"/>
+      <c r="B8" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="17"/>
+      <c r="I8" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="K8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L8" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="M8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="N8" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="O8" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="R8" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="S8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="T8" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="U8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="V8" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="W8" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="X8" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y8" s="10"/>
+    </row>
+    <row r="9" spans="1:25" ht="30" customHeight="1">
+      <c r="A9" s="13"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="10"/>
+      <c r="S9" s="10"/>
+      <c r="T9" s="10"/>
+      <c r="U9" s="10"/>
+      <c r="V9" s="10"/>
+      <c r="W9" s="10"/>
+      <c r="X9" s="10"/>
+      <c r="Y9" s="10"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>